<commit_message>
Attempting to submit to JLCPCB
</commit_message>
<xml_diff>
--- a/PCB/Waveform Generator/assembly/BOM.xlsx
+++ b/PCB/Waveform Generator/assembly/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nanodyn-my.sharepoint.com/personal/nicholas_nanodyn_co_za/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nanodyn-my.sharepoint.com/personal/nicholas_nanodyn_co_za/Documents/Desktop/GIT repository/Waveform-generator/PCB/Waveform Generator/assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A458C5A2C35038D7FB7FC123FFAC3D5C2DCA8074" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FD4457B3-594E-4FB6-91EF-B9A29AAE4FB4}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="11_A458C5A2C35038D7FB7FC123FFAC3D5C2DCA8074" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C3477C2E-4104-4B14-9EAC-E2E93DFB4163}"/>
   <bookViews>
-    <workbookView xWindow="-9855" yWindow="-15945" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9855" yWindow="-16770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="137">
   <si>
     <t>Comment</t>
   </si>
@@ -102,9 +102,6 @@
     <t xml:space="preserve">BTN3, </t>
   </si>
   <si>
-    <t>10n</t>
-  </si>
-  <si>
     <t xml:space="preserve">C1, C2, </t>
   </si>
   <si>
@@ -117,69 +114,45 @@
     <t>C57112</t>
   </si>
   <si>
-    <t>10u</t>
-  </si>
-  <si>
     <t xml:space="preserve">C7, C10, </t>
   </si>
   <si>
     <t>C19702</t>
   </si>
   <si>
-    <t>0.1u</t>
-  </si>
-  <si>
     <t xml:space="preserve">C8, C9, </t>
   </si>
   <si>
-    <t>12p</t>
-  </si>
-  <si>
     <t xml:space="preserve">C11, C12, C13, C24, </t>
   </si>
   <si>
     <t>C1547</t>
   </si>
   <si>
-    <t>4u7</t>
-  </si>
-  <si>
     <t xml:space="preserve">C14, </t>
   </si>
   <si>
     <t>C23733</t>
   </si>
   <si>
-    <t>100n</t>
-  </si>
-  <si>
     <t xml:space="preserve">C15, C16, C17, C18, C19, C31, </t>
   </si>
   <si>
     <t>C1525</t>
   </si>
   <si>
-    <t>1u</t>
-  </si>
-  <si>
     <t xml:space="preserve">C20, C21, </t>
   </si>
   <si>
     <t>C52923</t>
   </si>
   <si>
-    <t>2.2u</t>
-  </si>
-  <si>
     <t xml:space="preserve">C22, C23, </t>
   </si>
   <si>
     <t>C12530</t>
   </si>
   <si>
-    <t>20p</t>
-  </si>
-  <si>
     <t xml:space="preserve">C25, C26, </t>
   </si>
   <si>
@@ -195,9 +168,6 @@
     <t>B5819W</t>
   </si>
   <si>
-    <t xml:space="preserve">D1, </t>
-  </si>
-  <si>
     <t>SOD-123</t>
   </si>
   <si>
@@ -207,27 +177,18 @@
     <t>BLUE</t>
   </si>
   <si>
-    <t xml:space="preserve">D4, D11, LED1, </t>
-  </si>
-  <si>
     <t>C72041</t>
   </si>
   <si>
     <t>300mA</t>
   </si>
   <si>
-    <t xml:space="preserve">F1, </t>
-  </si>
-  <si>
     <t>C207010</t>
   </si>
   <si>
     <t>100 @ 100MHz</t>
   </si>
   <si>
-    <t xml:space="preserve">FB1, FB2, </t>
-  </si>
-  <si>
     <t>C1023</t>
   </si>
   <si>
@@ -258,27 +219,18 @@
     <t>RED</t>
   </si>
   <si>
-    <t xml:space="preserve">LED2, LED4, </t>
-  </si>
-  <si>
     <t>C2286</t>
   </si>
   <si>
     <t>GREEN</t>
   </si>
   <si>
-    <t xml:space="preserve">LED3, LED5, PWR1, PWR2, PWR3, </t>
-  </si>
-  <si>
     <t>C72043</t>
   </si>
   <si>
     <t>AMS1117-3.3</t>
   </si>
   <si>
-    <t xml:space="preserve">PS2, </t>
-  </si>
-  <si>
     <t>SOT-223</t>
   </si>
   <si>
@@ -288,9 +240,6 @@
     <t>AO3401A</t>
   </si>
   <si>
-    <t xml:space="preserve">Q0, </t>
-  </si>
-  <si>
     <t>SOT-23</t>
   </si>
   <si>
@@ -300,75 +249,42 @@
     <t>Q_NPN_BCE</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1, Q2, Q4, Q5, Q6, Q7, Q8, </t>
-  </si>
-  <si>
     <t>C2150</t>
   </si>
   <si>
     <t>Q_PNP_BCE</t>
   </si>
   <si>
-    <t xml:space="preserve">Q3, </t>
-  </si>
-  <si>
     <t>C8542</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R2, R3, R4, R7, R11, R15, R16, R17, R18, </t>
-  </si>
-  <si>
     <t>C11702</t>
   </si>
   <si>
     <t>10k</t>
   </si>
   <si>
-    <t xml:space="preserve">R5, R13, R14, R19, R20, </t>
-  </si>
-  <si>
     <t>C25744</t>
   </si>
   <si>
-    <t xml:space="preserve">R6, R8, R35, R36, </t>
-  </si>
-  <si>
     <t>C21190</t>
   </si>
   <si>
     <t>C23182</t>
   </si>
   <si>
-    <t xml:space="preserve">R10, R21, R22, R24, R26, R28, </t>
-  </si>
-  <si>
     <t>C23179</t>
   </si>
   <si>
     <t>C25118</t>
   </si>
   <si>
-    <t xml:space="preserve">R23, R25, R27, R37, R38, </t>
-  </si>
-  <si>
     <t>C25105</t>
   </si>
   <si>
-    <t xml:space="preserve">R29, R30, R31, R32, </t>
-  </si>
-  <si>
     <t>C25092</t>
   </si>
   <si>
-    <t>2k2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R33, R34, </t>
-  </si>
-  <si>
     <t>C25879</t>
   </si>
   <si>
@@ -378,30 +294,15 @@
     <t>SW_SPDT</t>
   </si>
   <si>
-    <t xml:space="preserve">SW1, SW2, SW3, </t>
-  </si>
-  <si>
     <t>C319019</t>
   </si>
   <si>
-    <t>STM32F427VITx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1, </t>
-  </si>
-  <si>
     <t>LQFP-100_14.0x14.0x0.5P</t>
   </si>
   <si>
-    <t>C57097</t>
-  </si>
-  <si>
     <t>MAX485EESAT</t>
   </si>
   <si>
-    <t xml:space="preserve">U2, </t>
-  </si>
-  <si>
     <t>SOIC-8_3.9x4.9x1.27P</t>
   </si>
   <si>
@@ -411,9 +312,6 @@
     <t>USBLC6-2SC6</t>
   </si>
   <si>
-    <t xml:space="preserve">U3, U6, U7, U9, U10, U11, </t>
-  </si>
-  <si>
     <t>SOT-23-6</t>
   </si>
   <si>
@@ -423,9 +321,6 @@
     <t>OPA1602</t>
   </si>
   <si>
-    <t xml:space="preserve">U4, U5, </t>
-  </si>
-  <si>
     <t>SOP-8_3.9x4.9x1.27P</t>
   </si>
   <si>
@@ -435,9 +330,6 @@
     <t>LM335ADT</t>
   </si>
   <si>
-    <t xml:space="preserve">U8, </t>
-  </si>
-  <si>
     <t>C361027</t>
   </si>
   <si>
@@ -451,6 +343,129 @@
   </si>
   <si>
     <t>C9006</t>
+  </si>
+  <si>
+    <t>C95448</t>
+  </si>
+  <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>4u7F</t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>20pF</t>
+  </si>
+  <si>
+    <t>1kΩ</t>
+  </si>
+  <si>
+    <t>47Ω</t>
+  </si>
+  <si>
+    <t>470Ω</t>
+  </si>
+  <si>
+    <t>33Ω</t>
+  </si>
+  <si>
+    <t>22Ω</t>
+  </si>
+  <si>
+    <t>2k2Ω</t>
+  </si>
+  <si>
+    <t>120Ω</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D4, D11, LED1</t>
+  </si>
+  <si>
+    <t>FB1, FB2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>LED2, LED4</t>
+  </si>
+  <si>
+    <t>LED3, LED5, PWR1, PWR2, PWR3</t>
+  </si>
+  <si>
+    <t>Q1, Q2, Q4, Q5, Q6, Q7, Q8</t>
+  </si>
+  <si>
+    <t>Q0</t>
+  </si>
+  <si>
+    <t>PS2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R7, R11, R15, R16, R17, R18</t>
+  </si>
+  <si>
+    <t>R5, R13, R14, R19, R20</t>
+  </si>
+  <si>
+    <t>R6, R8, R35, R36</t>
+  </si>
+  <si>
+    <t>R10, R21, R22, R24, R26, R28</t>
+  </si>
+  <si>
+    <t>R23, R25, R27, R37, R38</t>
+  </si>
+  <si>
+    <t>R29, R30, R31, R32</t>
+  </si>
+  <si>
+    <t>R33, R34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SW1, SW2, SW3 </t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3, U6, U7, U9, U10, U11</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>U4, U5</t>
+  </si>
+  <si>
+    <t>STM32F429VGT6</t>
   </si>
 </sst>
 </file>
@@ -531,7 +546,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -546,6 +561,9 @@
     </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,7 +843,7 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -852,621 +870,622 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.95" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
+        <v>114</v>
+      </c>
+      <c r="C3" s="3">
+        <v>603</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
+        <v>116</v>
+      </c>
+      <c r="C4" s="3">
+        <v>603</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>115</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1206</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1206</v>
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3">
-        <v>603</v>
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C8" s="3">
         <v>603</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>118</v>
       </c>
       <c r="C9" s="3">
         <v>603</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="3">
-        <v>402</v>
+        <v>121</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3">
-        <v>402</v>
+        <v>120</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3">
-        <v>402</v>
+        <v>119</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="3">
-        <v>402</v>
+        <v>122</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>123</v>
       </c>
       <c r="C14" s="3">
         <v>402</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="C15" s="3">
         <v>402</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
       <c r="C16" s="3">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>107</v>
+      </c>
+      <c r="B17" s="4">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3">
+        <v>603</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>50</v>
+        <v>126</v>
       </c>
       <c r="C18" s="3">
         <v>603</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>53</v>
+        <v>107</v>
+      </c>
+      <c r="B19" s="4">
+        <v>12</v>
       </c>
       <c r="C19" s="3">
-        <v>603</v>
+        <v>402</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>56</v>
+        <v>127</v>
       </c>
       <c r="C20" s="3">
-        <v>1206</v>
+        <v>402</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>60</v>
+        <v>128</v>
+      </c>
+      <c r="C21" s="3">
+        <v>402</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>62</v>
+        <v>111</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>129</v>
+      </c>
+      <c r="C22" s="3">
+        <v>402</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="3">
-        <v>603</v>
+        <v>130</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>69</v>
+        <v>136</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="3">
-        <v>603</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>71</v>
+        <v>131</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" s="3">
-        <v>402</v>
+        <v>93</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>90</v>
+        <v>112</v>
+      </c>
+      <c r="B30" s="4">
+        <v>39</v>
       </c>
       <c r="C30" s="3">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>86</v>
+        <v>5</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C31" s="3">
+        <v>6</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1206</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="3">
         <v>603</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3">
-        <v>47</v>
-      </c>
-      <c r="B32" s="4">
-        <v>9</v>
-      </c>
-      <c r="C32" s="3">
-        <v>603</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="3">
-        <v>470</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="3">
-        <v>603</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="3">
-        <v>47</v>
-      </c>
-      <c r="B34" s="4">
-        <v>12</v>
-      </c>
-      <c r="C34" s="3">
-        <v>402</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="3">
-        <v>33</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="3">
-        <v>402</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="3">
-        <v>22</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="3">
-        <v>402</v>
-      </c>
       <c r="D36" s="3" t="s">
-        <v>101</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>103</v>
+        <v>19</v>
       </c>
       <c r="C37" s="3">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="3">
-        <v>120</v>
-      </c>
-      <c r="B38" s="4">
-        <v>39</v>
+      <c r="A38" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C38" s="3">
         <v>603</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="C39" s="3">
+        <v>402</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>111</v>
+        <v>24</v>
+      </c>
+      <c r="C40" s="3">
+        <v>402</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>112</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>115</v>
+        <v>26</v>
+      </c>
+      <c r="C41" s="3">
+        <v>402</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>116</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>119</v>
+        <v>28</v>
+      </c>
+      <c r="C42" s="3">
+        <v>402</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>120</v>
+        <v>29</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>123</v>
+        <v>30</v>
+      </c>
+      <c r="C43" s="3">
+        <v>402</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>115</v>
+        <v>32</v>
+      </c>
+      <c r="C44" s="3">
+        <v>402</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>127</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>130</v>
+        <v>34</v>
+      </c>
+      <c r="C45" s="3">
+        <v>402</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>131</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Trying to order from JLCPCB
</commit_message>
<xml_diff>
--- a/PCB/Waveform Generator/assembly/BOM.xlsx
+++ b/PCB/Waveform Generator/assembly/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nanodyn-my.sharepoint.com/personal/nicholas_nanodyn_co_za/Documents/Desktop/GIT repository/Waveform-generator/PCB/Waveform Generator/assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="11_A458C5A2C35038D7FB7FC123FFAC3D5C2DCA8074" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C3477C2E-4104-4B14-9EAC-E2E93DFB4163}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_A458C5A2C35038D7FB7FC123FFAC3D5C2DCA8074" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1B029F54-0E4B-4073-A569-B1EDED51DF61}"/>
   <bookViews>
     <workbookView xWindow="-9855" yWindow="-16770" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,44 +31,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>LCSC Part #</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>（</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <charset val="134"/>
-      </rPr>
-      <t>optional</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>）</t>
-    </r>
-  </si>
-  <si>
     <t>C14663</t>
   </si>
   <si>
@@ -466,6 +428,9 @@
   </si>
   <si>
     <t>STM32F429VGT6</t>
+  </si>
+  <si>
+    <t>LCSC Part #（optional）</t>
   </si>
 </sst>
 </file>
@@ -475,7 +440,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;R&quot;#,##0;[Red]\-&quot;R&quot;#,##0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,23 +449,19 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -550,19 +511,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -843,12 +804,12 @@
   <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
@@ -865,222 +826,222 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.95" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="3">
         <v>603</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="3">
         <v>603</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="3">
         <v>1206</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="3">
         <v>603</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="3">
         <v>603</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" s="3">
         <v>402</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C15" s="3">
         <v>402</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="3">
         <v>603</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="4">
         <v>9</v>
@@ -1089,26 +1050,26 @@
         <v>603</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="3">
         <v>603</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B19" s="4">
         <v>12</v>
@@ -1117,152 +1078,152 @@
         <v>402</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="3">
         <v>402</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="3">
         <v>402</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="3">
         <v>402</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C25" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="4">
         <v>39</v>
@@ -1271,217 +1232,217 @@
         <v>603</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C35" s="3">
         <v>1206</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C36" s="3">
         <v>603</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37" s="3">
         <v>603</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" s="3">
         <v>603</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C39" s="3">
         <v>402</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="3">
         <v>402</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="3">
         <v>402</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42" s="3">
         <v>402</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" s="3">
         <v>402</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C44" s="3">
         <v>402</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C45" s="3">
         <v>402</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>